<commit_message>
docs: se edita el doc de deck_propio
</commit_message>
<xml_diff>
--- a/docs/deck_propio.xlsx
+++ b/docs/deck_propio.xlsx
@@ -24,78 +24,111 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
-  <si>
-    <t>Carta,Utilidad,Cantidad</t>
-  </si>
-  <si>
-    <t>Effect Veiler,Defensive,3</t>
-  </si>
-  <si>
-    <t>Rescue-ACE Hydrant, Starter,2</t>
-  </si>
-  <si>
-    <t>Snake-Eyes Poplar,Starter,2</t>
-  </si>
-  <si>
-    <t>Maxx C,Defensive,3</t>
-  </si>
-  <si>
-    <t>Ash Blossom &amp; Joyous Springs,Defensive,3</t>
-  </si>
-  <si>
-    <t>Rescue-ACE Impulse,Defensive,2</t>
-  </si>
-  <si>
-    <t>Rescue-ACE Air Lifter, Starter,2</t>
-  </si>
-  <si>
-    <t>Rescue-ACE Fire Attacker, Garnet,1</t>
-  </si>
-  <si>
-    <t>Rescue-ACE Fire Engine,Garnet,1</t>
-  </si>
-  <si>
-    <t>Diabellstar the Black Witch, Starter,2</t>
-  </si>
-  <si>
-    <t>Rescue-ACE Preventer,Combo piece,2</t>
-  </si>
-  <si>
-    <t>Rescue-ACE Turbulunce, Combo piece,2</t>
-  </si>
-  <si>
-    <t>Bonfire,Starter,3</t>
-  </si>
-  <si>
-    <t>Original Sinful Spoils - Snake-Eye, Combo piece,2</t>
-  </si>
-  <si>
-    <t>Rescue-ACE HQ, Garnet,1</t>
-  </si>
-  <si>
-    <t>Called by the Grave,Defensive,2</t>
-  </si>
-  <si>
-    <t>RESCUE!,Extender,1</t>
-  </si>
-  <si>
-    <t>ALERT!, Extender,1</t>
-  </si>
-  <si>
-    <t>EMERGENCY!,Extender,3</t>
-  </si>
-  <si>
-    <t>WANTED: Seeker of Sinful Spoils, Starter,1</t>
-  </si>
-  <si>
-    <t>CONTAIN!,Garnet,1</t>
-  </si>
-  <si>
-    <t>EXTINGUISH!, Garnet,1</t>
-  </si>
-  <si>
-    <t>Sinful Spoils of Betrayal - Silvera, Garnet,1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+  <si>
+    <t>Snake-Eyes Poplar</t>
+  </si>
+  <si>
+    <t>Starter</t>
+  </si>
+  <si>
+    <t>Maxx C</t>
+  </si>
+  <si>
+    <t>Defensive</t>
+  </si>
+  <si>
+    <t>Ash Blossom &amp; Joyous Springs</t>
+  </si>
+  <si>
+    <t>Rescue-ACE Impulse</t>
+  </si>
+  <si>
+    <t>Rescue-ACE Air Lifter</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Starter</t>
+  </si>
+  <si>
+    <t>Rescue-ACE Fire Attacker</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Garnet</t>
+  </si>
+  <si>
+    <t>Rescue-ACE Fire Engine</t>
+  </si>
+  <si>
+    <t>Garnet</t>
+  </si>
+  <si>
+    <t>Diabellstar the Black Witch</t>
+  </si>
+  <si>
+    <t>Rescue-ACE Preventer</t>
+  </si>
+  <si>
+    <t>Combo piece</t>
+  </si>
+  <si>
+    <t>Rescue-ACE Turbulunce</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Combo piece</t>
+  </si>
+  <si>
+    <t>Bonfire</t>
+  </si>
+  <si>
+    <t>Original Sinful Spoils - Snake-Eye</t>
+  </si>
+  <si>
+    <t>Rescue-ACE HQ</t>
+  </si>
+  <si>
+    <t>Called by the Grave</t>
+  </si>
+  <si>
+    <t>RESCUE!</t>
+  </si>
+  <si>
+    <t>Extender</t>
+  </si>
+  <si>
+    <t>ALERT!</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Extender</t>
+  </si>
+  <si>
+    <t>EMERGENCY!</t>
+  </si>
+  <si>
+    <t>WANTED: Seeker of Sinful Spoils</t>
+  </si>
+  <si>
+    <t>CONTAIN!</t>
+  </si>
+  <si>
+    <t>EXTINGUISH!</t>
+  </si>
+  <si>
+    <t>Sinful Spoils of Betrayal - Silvera</t>
+  </si>
+  <si>
+    <t>Carta</t>
+  </si>
+  <si>
+    <t>Utilidad</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
+  </si>
+  <si>
+    <t>Effect Veiler</t>
+  </si>
+  <si>
+    <t>Rescue-ACE Hydrant</t>
   </si>
 </sst>
 </file>
@@ -413,132 +446,276 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A24"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>29</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: se corrigen errores de digitación en los valores del excel
</commit_message>
<xml_diff>
--- a/docs/deck_propio.xlsx
+++ b/docs/deck_propio.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>Snake-Eyes Poplar</t>
   </si>
@@ -47,15 +47,9 @@
     <t>Rescue-ACE Air Lifter</t>
   </si>
   <si>
-    <t xml:space="preserve"> Starter</t>
-  </si>
-  <si>
     <t>Rescue-ACE Fire Attacker</t>
   </si>
   <si>
-    <t xml:space="preserve"> Garnet</t>
-  </si>
-  <si>
     <t>Rescue-ACE Fire Engine</t>
   </si>
   <si>
@@ -74,9 +68,6 @@
     <t>Rescue-ACE Turbulunce</t>
   </si>
   <si>
-    <t xml:space="preserve"> Combo piece</t>
-  </si>
-  <si>
     <t>Bonfire</t>
   </si>
   <si>
@@ -96,9 +87,6 @@
   </si>
   <si>
     <t>ALERT!</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Extender</t>
   </si>
   <si>
     <t>EMERGENCY!</t>
@@ -448,26 +436,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -478,10 +466,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -536,7 +524,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -544,7 +532,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -555,10 +543,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -566,10 +554,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -577,10 +565,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -588,10 +576,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -599,7 +587,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
@@ -610,10 +598,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -621,7 +609,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
@@ -632,7 +620,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
@@ -643,10 +631,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -654,10 +642,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -665,10 +653,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C20">
         <v>3</v>
@@ -676,10 +664,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -687,10 +675,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -698,7 +686,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
@@ -709,7 +697,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>

</xml_diff>